<commit_message>
update covid graph and region_countries threshold
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_regions_countries.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_regions_countries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -27,7 +27,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-10-15 13:17:46</t>
+    <t xml:space="preserve">2021-10-15 15:19:26</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -361,6 +361,18 @@
   </si>
   <si>
     <t xml:space="preserve">VNM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRA</t>
   </si>
 </sst>
 </file>
@@ -2613,6 +2625,52 @@
         <v>0.624526121278409</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-3.13681919422224</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.149748265115072</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6.74437083964458</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.145332580540567</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1.62051639729969</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.0707187356488979</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.63879934291407</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.144843896816565</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>